<commit_message>
added out query system
</commit_message>
<xml_diff>
--- a/Nado Game/pyqt5/자재관리/사용대장.xlsx
+++ b/Nado Game/pyqt5/자재관리/사용대장.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\source\pygame\Nado Game\pyqt5\자재관리\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48139A2-0807-4E18-9267-62D29EA118E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="18990" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>사용일</t>
   </si>
@@ -119,17 +125,21 @@
   </si>
   <si>
     <t>111</t>
+  </si>
+  <si>
+    <t>품목누계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,8 +147,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -184,15 +201,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -234,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,9 +291,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,6 +343,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,14 +536,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,10 +571,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -531,10 +600,13 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -557,10 +629,13 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -583,10 +658,13 @@
         <v>30</v>
       </c>
       <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -609,10 +687,13 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -635,10 +716,13 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -661,10 +745,13 @@
         <v>31</v>
       </c>
       <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -687,10 +774,13 @@
         <v>31</v>
       </c>
       <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -713,10 +803,13 @@
         <v>31</v>
       </c>
       <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -739,10 +832,13 @@
         <v>31</v>
       </c>
       <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -765,10 +861,13 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -791,10 +890,15 @@
         <v>31</v>
       </c>
       <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>